<commit_message>
still working, up through excavation costs. Next is concrete cost
</commit_message>
<xml_diff>
--- a/dev/fluor/point375inch_pipe.xlsx
+++ b/dev/fluor/point375inch_pipe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\jamar1391.github.io\dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\jamar1391.github.io\dev\fluor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E75D28-1813-484C-AC83-889B8E70EFA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EE6155-37DB-47CF-8015-0EA364F057CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="19944" windowHeight="10980" activeTab="7" xr2:uid="{F22476ED-52B1-4252-BA3D-E6827F3736A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{F22476ED-52B1-4252-BA3D-E6827F3736A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet10" sheetId="10" r:id="rId1"/>
@@ -528,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE3189A-26F2-40A0-95DF-522BA0E109A0}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
@@ -5136,7 +5136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5C9D9B-ED2E-4EF2-8C6C-CAB5C62ADD28}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -8587,8 +8587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C244507-49DC-48CB-8360-D920A51B899D}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
location costs quantified; still need location-based pipe sizing
</commit_message>
<xml_diff>
--- a/dev/fluor/point375inch_pipe.xlsx
+++ b/dev/fluor/point375inch_pipe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\jamar1391.github.io\dev\fluor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joe/dev/hello-world/dev/fluor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EE6155-37DB-47CF-8015-0EA364F057CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865C67DE-8598-C848-B90F-9495B7504323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{F22476ED-52B1-4252-BA3D-E6827F3736A8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26760" windowHeight="14500" activeTab="7" xr2:uid="{F22476ED-52B1-4252-BA3D-E6827F3736A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet10" sheetId="10" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -528,16 +528,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE3189A-26F2-40A0-95DF-522BA0E109A0}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +575,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -613,7 +613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -663,7 +663,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -713,7 +713,7 @@
         <v>104.96</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -763,7 +763,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -813,7 +813,7 @@
         <v>950.66</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -863,7 +863,7 @@
         <v>714.89</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -913,7 +913,7 @@
         <v>555.9</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -963,7 +963,7 @@
         <v>363.39</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>310.39999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>279.02999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>55.15</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>-41.11</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>-601.32000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
@@ -1682,12 +1682,13 @@
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1725,7 +1726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1763,7 +1764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1863,7 +1864,7 @@
         <v>104.96</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1913,7 +1914,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1963,7 +1964,7 @@
         <v>950.66</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2013,7 +2014,7 @@
         <v>1724.83</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2063,7 +2064,7 @@
         <v>1565.84</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2113,7 +2114,7 @@
         <v>1373.33</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2163,7 +2164,7 @@
         <v>1320.33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>1288.96</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2263,7 +2264,7 @@
         <v>1065.08</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2313,7 +2314,7 @@
         <v>968.83</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2363,7 +2364,7 @@
         <v>408.61</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -2442,7 +2443,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2500,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2529,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -2558,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2587,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -2645,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -2674,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -2703,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -2732,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -2761,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -2790,7 +2791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
@@ -2819,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -2837,15 +2838,15 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:P16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2883,7 +2884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2921,7 +2922,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2971,7 +2972,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3021,7 +3022,7 @@
         <v>104.96</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3071,7 +3072,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3121,7 +3122,7 @@
         <v>950.66</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>714.89</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>1565.84</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3271,7 +3272,7 @@
         <v>1373.33</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -3321,7 +3322,7 @@
         <v>1320.33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3371,7 +3372,7 @@
         <v>1288.96</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3421,7 +3422,7 @@
         <v>1065.08</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3471,7 +3472,7 @@
         <v>968.83</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3521,7 +3522,7 @@
         <v>408.61</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3571,7 +3572,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -3600,7 +3601,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3658,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -3687,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -3716,7 +3717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -3745,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -3774,7 +3775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -3803,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -3890,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -3919,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -3948,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
@@ -3990,12 +3991,12 @@
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4033,7 +4034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4071,7 +4072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4171,7 +4172,7 @@
         <v>104.96</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -4221,7 +4222,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -4271,7 +4272,7 @@
         <v>950.66</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -4321,7 +4322,7 @@
         <v>714.89</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -4371,7 +4372,7 @@
         <v>555.9</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -4421,7 +4422,7 @@
         <v>1373.33</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -4471,7 +4472,7 @@
         <v>1320.33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -4521,7 +4522,7 @@
         <v>1288.96</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -4571,7 +4572,7 @@
         <v>1065.08</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -4621,7 +4622,7 @@
         <v>968.83</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -4671,7 +4672,7 @@
         <v>408.61</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -4721,7 +4722,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -4750,7 +4751,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -4779,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -4808,7 +4809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -4837,7 +4838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -4866,7 +4867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -4895,7 +4896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -4924,7 +4925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -4953,7 +4954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -4982,7 +4983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -5011,7 +5012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -5040,7 +5041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -5069,7 +5070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -5098,7 +5099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
@@ -5136,16 +5137,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5C9D9B-ED2E-4EF2-8C6C-CAB5C62ADD28}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5183,7 +5184,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5221,7 +5222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -5271,7 +5272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5321,7 +5322,7 @@
         <v>104.96</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -5371,7 +5372,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -5421,7 +5422,7 @@
         <v>950.66</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -5471,7 +5472,7 @@
         <v>714.89</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -5521,7 +5522,7 @@
         <v>555.9</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -5571,7 +5572,7 @@
         <v>363.39</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -5621,7 +5622,7 @@
         <v>1320.33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -5671,7 +5672,7 @@
         <v>1288.96</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -5721,7 +5722,7 @@
         <v>1065.08</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -5771,7 +5772,7 @@
         <v>968.83</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -5821,7 +5822,7 @@
         <v>408.61</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -5871,7 +5872,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -5900,7 +5901,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -5929,7 +5930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -5958,7 +5959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -5987,7 +5988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -6016,7 +6017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -6045,7 +6046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -6074,7 +6075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -6103,7 +6104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -6132,7 +6133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -6161,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -6190,7 +6191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -6219,7 +6220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -6248,7 +6249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
@@ -6290,12 +6291,12 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6333,7 +6334,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6371,7 +6372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -6421,7 +6422,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -6471,7 +6472,7 @@
         <v>104.96</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -6521,7 +6522,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -6571,7 +6572,7 @@
         <v>950.66</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -6621,7 +6622,7 @@
         <v>714.89</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -6671,7 +6672,7 @@
         <v>555.9</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -6721,7 +6722,7 @@
         <v>363.39</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -6771,7 +6772,7 @@
         <v>310.39999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -6821,7 +6822,7 @@
         <v>1288.96</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -6871,7 +6872,7 @@
         <v>1065.08</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -6921,7 +6922,7 @@
         <v>968.83</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -6971,7 +6972,7 @@
         <v>408.61</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -7021,7 +7022,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -7050,7 +7051,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -7079,7 +7080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -7108,7 +7109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -7137,7 +7138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -7166,7 +7167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -7195,7 +7196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -7224,7 +7225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -7253,7 +7254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -7282,7 +7283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -7311,7 +7312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -7340,7 +7341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -7369,7 +7370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -7398,7 +7399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
@@ -7440,13 +7441,13 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7484,7 +7485,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7522,7 +7523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -7572,7 +7573,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -7622,7 +7623,7 @@
         <v>104.96</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -7672,7 +7673,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -7722,7 +7723,7 @@
         <v>950.66</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -7772,7 +7773,7 @@
         <v>714.89</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -7822,7 +7823,7 @@
         <v>555.9</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -7872,7 +7873,7 @@
         <v>363.39</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -7922,7 +7923,7 @@
         <v>310.39999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -7972,7 +7973,7 @@
         <v>279.02999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -8022,7 +8023,7 @@
         <v>1065.08</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -8072,7 +8073,7 @@
         <v>968.83</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -8122,7 +8123,7 @@
         <v>408.61</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -8172,7 +8173,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -8201,7 +8202,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -8230,7 +8231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -8259,7 +8260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -8288,7 +8289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -8317,7 +8318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -8346,7 +8347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -8375,7 +8376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -8404,7 +8405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -8433,7 +8434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -8462,7 +8463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -8491,7 +8492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -8520,7 +8521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -8549,7 +8550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
@@ -8587,20 +8588,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C244507-49DC-48CB-8360-D920A51B899D}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8638,7 +8639,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -8676,7 +8677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -8726,7 +8727,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -8776,7 +8777,7 @@
         <v>104.96</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -8826,7 +8827,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -8876,7 +8877,7 @@
         <v>950.66</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -8926,7 +8927,7 @@
         <v>714.89</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -8976,7 +8977,7 @@
         <v>555.9</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -9026,7 +9027,7 @@
         <v>363.39</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -9076,7 +9077,7 @@
         <v>310.39999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -9126,7 +9127,7 @@
         <v>279.02999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -9176,7 +9177,7 @@
         <v>55.15</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -9226,7 +9227,7 @@
         <v>968.83</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -9276,7 +9277,7 @@
         <v>408.61</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -9326,7 +9327,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -9355,7 +9356,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -9384,7 +9385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -9413,7 +9414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -9442,7 +9443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -9471,7 +9472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -9500,7 +9501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -9529,7 +9530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -9558,7 +9559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -9587,7 +9588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -9616,7 +9617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -9645,7 +9646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -9674,7 +9675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -9703,7 +9704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
@@ -9745,12 +9746,12 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9788,7 +9789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -9826,7 +9827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -9876,7 +9877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -9926,7 +9927,7 @@
         <v>104.96</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -9976,7 +9977,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -10026,7 +10027,7 @@
         <v>950.66</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -10076,7 +10077,7 @@
         <v>714.89</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -10126,7 +10127,7 @@
         <v>555.9</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -10176,7 +10177,7 @@
         <v>363.39</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -10226,7 +10227,7 @@
         <v>310.39999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -10276,7 +10277,7 @@
         <v>279.02999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -10326,7 +10327,7 @@
         <v>55.15</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -10376,7 +10377,7 @@
         <v>-41.11</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -10426,7 +10427,7 @@
         <v>408.61</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -10476,7 +10477,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -10505,7 +10506,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -10534,7 +10535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -10572,7 +10573,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -10601,7 +10602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -10630,7 +10631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -10659,7 +10660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -10688,7 +10689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -10717,7 +10718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -10746,7 +10747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -10775,7 +10776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -10804,7 +10805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -10833,7 +10834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -10862,7 +10863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>

</xml_diff>